<commit_message>
removed unwanted projects, added new code for Excel.
</commit_message>
<xml_diff>
--- a/SpreadSheetLightVb1/bin/Debug/ExcelFiles/DemoExport.xlsx
+++ b/SpreadSheetLightVb1/bin/Debug/ExcelFiles/DemoExport.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Info_Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Info_Table" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,10 +19,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Your header</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -55,9 +72,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,19 +356,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:A12"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="7:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="7:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="7:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="7:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="7:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>